<commit_message>
small changes to estimation algorithm
</commit_message>
<xml_diff>
--- a/Figures/Table_2.xlsx
+++ b/Figures/Table_2.xlsx
@@ -13,7 +13,187 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="75">
+  <si>
+    <t>VarNames</t>
+  </si>
+  <si>
+    <t>Population 1920s</t>
+  </si>
+  <si>
+    <t>Population 1930s</t>
+  </si>
+  <si>
+    <t>Population 1940s</t>
+  </si>
+  <si>
+    <t>Population Density 1920s</t>
+  </si>
+  <si>
+    <t>Population Density 1930s</t>
+  </si>
+  <si>
+    <t>Population Density 1940s</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>VarNames</t>
+  </si>
+  <si>
+    <t>Population 1920s</t>
+  </si>
+  <si>
+    <t>Population 1930s</t>
+  </si>
+  <si>
+    <t>Population 1940s</t>
+  </si>
+  <si>
+    <t>Population Density 1920s</t>
+  </si>
+  <si>
+    <t>Population Density 1930s</t>
+  </si>
+  <si>
+    <t>Population Density 1940s</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>VarNames</t>
+  </si>
+  <si>
+    <t>Population 1920s</t>
+  </si>
+  <si>
+    <t>Population 1930s</t>
+  </si>
+  <si>
+    <t>Population 1940s</t>
+  </si>
+  <si>
+    <t>Population Density 1920s</t>
+  </si>
+  <si>
+    <t>Population Density 1930s</t>
+  </si>
+  <si>
+    <t>Population Density 1940s</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>VarNames</t>
+  </si>
+  <si>
+    <t>Population 1920s</t>
+  </si>
+  <si>
+    <t>Population 1930s</t>
+  </si>
+  <si>
+    <t>Population 1940s</t>
+  </si>
+  <si>
+    <t>Population Density 1920s</t>
+  </si>
+  <si>
+    <t>Population Density 1930s</t>
+  </si>
+  <si>
+    <t>Population Density 1940s</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
   <si>
     <t>VarNames</t>
   </si>
@@ -78,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -116,11 +296,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -152,6 +336,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,183 +365,190 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+        <v>61</v>
+      </c>
+      <c r="B2" s="0">
         <v>422130.20000000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>947923.19999999995</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>219894.39999999999</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1079858.3999999999</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>837594.90000000002</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>4540000.2999999998</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>749970</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>519223.90000000002</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0">
         <v>425201.79999999999</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>1023811.1111111111</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>222657.79999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>1088828.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>858783.09999999998</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>4230295.4000000004</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>746974</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>517967</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="B4" s="0">
         <v>442934.70000000001</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>1053156.6666666667</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>227860.70000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>1089367.7</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>720112.09999999998</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>2863548</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>641040</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>492093</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0">
         <v>21.159584187104514</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>20.649999999999999</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>51</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>40.044444444444451</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="0"/>
+      <c r="H5" s="0">
         <v>34.799999999999997</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>16.625</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
+        <v>65</v>
+      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0">
         <v>20.040692055928247</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>17.990000000000002</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>35.299999999999997</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>32</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="0"/>
+      <c r="H6" s="0">
         <v>28.5</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>13.800000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
+        <v>66</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0">
         <v>20.511553856096693</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>16.850000000000001</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>26.888888888888889</v>
       </c>
-      <c r="H7">
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0">
         <v>23.875</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>12.5</v>
       </c>
     </row>

</xml_diff>